<commit_message>
Removed video from lesson 9 and took out mattress plan terminology
Removed video from lesson 9 and took out mattress plan terminology
</commit_message>
<xml_diff>
--- a/ExcelFiles/CarLoanCaseStudy.xlsx
+++ b/ExcelFiles/CarLoanCaseStudy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/curtisgn_byui_edu/Documents/Course Lead/108/Math108XWebsite/math108x/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_2DCAAFA00C70649DC914E05F07606DEE53A881BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC43717C-7D05-4EE2-BEE2-43A63A879352}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_2DCAAFA00C70649DC914E05F07606DEE53A881BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8BB1F29-ADBD-4D3F-90CB-EB5C4B24ED1D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1118,7 +1118,7 @@
 </t>
   </si>
   <si>
-    <t>Winter 2023</t>
+    <t>Spring 2023</t>
   </si>
 </sst>
 </file>
@@ -3179,68 +3179,49 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="71" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3287,24 +3268,6 @@
     <xf numFmtId="0" fontId="35" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3317,28 +3280,150 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="12" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="51" fillId="9" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="51" fillId="9" borderId="68" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="69" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3348,17 +3433,11 @@
     </xf>
     <xf numFmtId="0" fontId="64" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="51" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="51" fillId="9" borderId="65" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -3370,9 +3449,6 @@
     <xf numFmtId="0" fontId="70" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -3380,82 +3456,6 @@
     <xf numFmtId="0" fontId="37" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="10" fontId="51" fillId="9" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="10" fontId="51" fillId="9" borderId="68" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="12" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -5217,21 +5217,21 @@
     <row r="2" spans="1:112" s="26" customFormat="1" ht="55.15" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="216" t="s">
+      <c r="C2" s="209" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="106"/>
-      <c r="I2" s="207" t="s">
+      <c r="I2" s="228" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
+      <c r="J2" s="228"/>
+      <c r="K2" s="228"/>
+      <c r="L2" s="228"/>
+      <c r="M2" s="228"/>
+      <c r="N2" s="228"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
       <c r="Q2" s="30"/>
@@ -5259,7 +5259,7 @@
       <c r="C4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="230" t="s">
+      <c r="D4" s="195" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="26"/>
@@ -5270,7 +5270,7 @@
       <c r="K4" s="27"/>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
-      <c r="N4" s="209" t="s">
+      <c r="N4" s="204" t="s">
         <v>24</v>
       </c>
       <c r="O4" s="37"/>
@@ -5290,10 +5290,10 @@
     <row r="5" spans="1:112" ht="22.15" customHeight="1">
       <c r="A5" s="9"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="231"/>
+      <c r="D5" s="197"/>
       <c r="F5" s="26"/>
       <c r="I5" s="2"/>
-      <c r="N5" s="209"/>
+      <c r="N5" s="204"/>
       <c r="O5" s="37"/>
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
@@ -5307,19 +5307,19 @@
       <c r="D6" s="22"/>
       <c r="F6" s="26"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="239" t="s">
+      <c r="J6" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="228" t="s">
+      <c r="N6" s="221" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="228"/>
-      <c r="P6" s="228"/>
-      <c r="Q6" s="228"/>
-      <c r="R6" s="228"/>
-      <c r="S6" s="228"/>
-      <c r="T6" s="228"/>
-      <c r="V6" s="239" t="s">
+      <c r="O6" s="221"/>
+      <c r="P6" s="221"/>
+      <c r="Q6" s="221"/>
+      <c r="R6" s="221"/>
+      <c r="S6" s="221"/>
+      <c r="T6" s="221"/>
+      <c r="V6" s="203" t="s">
         <v>39</v>
       </c>
       <c r="AC6" s="24"/>
@@ -5329,40 +5329,40 @@
       <c r="C7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="230" t="s">
+      <c r="D7" s="195" t="s">
         <v>64</v>
       </c>
       <c r="F7" s="26"/>
-      <c r="H7" s="234" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="234"/>
-      <c r="J7" s="239"/>
+      <c r="H7" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="205"/>
+      <c r="J7" s="203"/>
       <c r="N7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="241"/>
-      <c r="P7" s="242"/>
+      <c r="O7" s="207"/>
+      <c r="P7" s="208"/>
       <c r="Q7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="241"/>
-      <c r="S7" s="242"/>
+      <c r="R7" s="207"/>
+      <c r="S7" s="208"/>
       <c r="T7" s="132"/>
-      <c r="V7" s="239"/>
-      <c r="X7" s="234" t="s">
+      <c r="V7" s="203"/>
+      <c r="X7" s="205" t="s">
         <v>1</v>
       </c>
-      <c r="Y7" s="234"/>
+      <c r="Y7" s="205"/>
       <c r="Z7" s="41"/>
       <c r="AC7" s="24"/>
     </row>
     <row r="8" spans="1:112" ht="22.15" customHeight="1" thickTop="1">
       <c r="A8" s="9"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="243"/>
-      <c r="H8" s="234"/>
-      <c r="I8" s="234"/>
+      <c r="D8" s="196"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="205"/>
       <c r="J8" s="79" t="s">
         <v>2</v>
       </c>
@@ -5370,21 +5370,21 @@
       <c r="N8" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="241"/>
-      <c r="P8" s="242"/>
+      <c r="O8" s="207"/>
+      <c r="P8" s="208"/>
       <c r="Q8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="241"/>
-      <c r="S8" s="242"/>
+      <c r="R8" s="207"/>
+      <c r="S8" s="208"/>
       <c r="T8" s="133"/>
       <c r="U8" s="3"/>
       <c r="V8" s="162"/>
       <c r="W8" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="X8" s="234"/>
-      <c r="Y8" s="234"/>
+      <c r="X8" s="205"/>
+      <c r="Y8" s="205"/>
       <c r="Z8" s="41"/>
       <c r="AC8" s="24"/>
     </row>
@@ -5392,28 +5392,28 @@
       <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="18"/>
-      <c r="D9" s="231"/>
+      <c r="D9" s="197"/>
       <c r="E9" s="13"/>
-      <c r="H9" s="234"/>
-      <c r="I9" s="234"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="205"/>
       <c r="J9" s="80" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="163"/>
-      <c r="N9" s="226"/>
-      <c r="O9" s="227"/>
-      <c r="P9" s="227"/>
-      <c r="Q9" s="227"/>
-      <c r="R9" s="227"/>
-      <c r="S9" s="227"/>
-      <c r="T9" s="227"/>
+      <c r="N9" s="219"/>
+      <c r="O9" s="220"/>
+      <c r="P9" s="220"/>
+      <c r="Q9" s="220"/>
+      <c r="R9" s="220"/>
+      <c r="S9" s="220"/>
+      <c r="T9" s="220"/>
       <c r="U9" s="3"/>
       <c r="V9" s="163"/>
       <c r="W9" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="X9" s="234"/>
-      <c r="Y9" s="234"/>
+      <c r="X9" s="205"/>
+      <c r="Y9" s="205"/>
       <c r="Z9" s="41"/>
       <c r="AC9" s="24"/>
     </row>
@@ -5424,30 +5424,30 @@
       <c r="D10" s="11"/>
       <c r="E10" s="13"/>
       <c r="F10" s="35"/>
-      <c r="H10" s="235" t="s">
+      <c r="H10" s="222" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="235"/>
+      <c r="I10" s="222"/>
       <c r="J10" s="80" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="163"/>
-      <c r="N10" s="224"/>
-      <c r="O10" s="224"/>
-      <c r="P10" s="224"/>
-      <c r="Q10" s="224"/>
-      <c r="R10" s="224"/>
-      <c r="S10" s="224"/>
-      <c r="T10" s="224"/>
+      <c r="N10" s="217"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="217"/>
+      <c r="Q10" s="217"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="217"/>
+      <c r="T10" s="217"/>
       <c r="U10" s="3"/>
       <c r="V10" s="163"/>
       <c r="W10" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="X10" s="240" t="s">
+      <c r="X10" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="Y10" s="240"/>
+      <c r="Y10" s="206"/>
       <c r="Z10" s="42"/>
       <c r="AC10" s="24"/>
     </row>
@@ -5457,32 +5457,32 @@
       <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="232" t="s">
+      <c r="D11" s="201" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="35"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="235"/>
-      <c r="I11" s="235"/>
+      <c r="H11" s="222"/>
+      <c r="I11" s="222"/>
       <c r="J11" s="80" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="163"/>
-      <c r="N11" s="225"/>
-      <c r="O11" s="225"/>
-      <c r="P11" s="225"/>
-      <c r="Q11" s="225"/>
-      <c r="R11" s="225"/>
-      <c r="S11" s="225"/>
-      <c r="T11" s="225"/>
+      <c r="N11" s="218"/>
+      <c r="O11" s="218"/>
+      <c r="P11" s="218"/>
+      <c r="Q11" s="218"/>
+      <c r="R11" s="218"/>
+      <c r="S11" s="218"/>
+      <c r="T11" s="218"/>
       <c r="U11" s="3"/>
       <c r="V11" s="163"/>
       <c r="W11" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="X11" s="240"/>
-      <c r="Y11" s="240"/>
+      <c r="X11" s="206"/>
+      <c r="Y11" s="206"/>
       <c r="Z11" s="42"/>
       <c r="AC11" s="24"/>
     </row>
@@ -5490,33 +5490,33 @@
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="19"/>
-      <c r="D12" s="233"/>
+      <c r="D12" s="202"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="195" t="s">
+      <c r="F12" s="239" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="245"/>
-      <c r="H12" s="235"/>
-      <c r="I12" s="235"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="222"/>
+      <c r="I12" s="222"/>
       <c r="J12" s="80" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="164"/>
-      <c r="N12" s="225"/>
-      <c r="O12" s="225"/>
-      <c r="P12" s="225"/>
-      <c r="Q12" s="225"/>
-      <c r="R12" s="225"/>
-      <c r="S12" s="225"/>
-      <c r="T12" s="225"/>
+      <c r="N12" s="218"/>
+      <c r="O12" s="218"/>
+      <c r="P12" s="218"/>
+      <c r="Q12" s="218"/>
+      <c r="R12" s="218"/>
+      <c r="S12" s="218"/>
+      <c r="T12" s="218"/>
       <c r="U12" s="3"/>
       <c r="V12" s="164"/>
       <c r="W12" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="X12" s="240"/>
-      <c r="Y12" s="240"/>
-      <c r="Z12" s="195" t="s">
+      <c r="X12" s="206"/>
+      <c r="Y12" s="206"/>
+      <c r="Z12" s="239" t="s">
         <v>73</v>
       </c>
       <c r="AC12" s="24"/>
@@ -5527,19 +5527,19 @@
       <c r="C13" s="18"/>
       <c r="D13" s="14"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="195"/>
-      <c r="G13" s="245"/>
+      <c r="F13" s="239"/>
+      <c r="G13" s="200"/>
       <c r="J13" s="80" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="165"/>
-      <c r="N13" s="225"/>
-      <c r="O13" s="225"/>
-      <c r="P13" s="225"/>
-      <c r="Q13" s="225"/>
-      <c r="R13" s="225"/>
-      <c r="S13" s="225"/>
-      <c r="T13" s="225"/>
+      <c r="N13" s="218"/>
+      <c r="O13" s="218"/>
+      <c r="P13" s="218"/>
+      <c r="Q13" s="218"/>
+      <c r="R13" s="218"/>
+      <c r="S13" s="218"/>
+      <c r="T13" s="218"/>
       <c r="U13" s="3"/>
       <c r="V13" s="165"/>
       <c r="W13" s="85" t="s">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="195"/>
+      <c r="Z13" s="239"/>
       <c r="AC13" s="24"/>
     </row>
     <row r="14" spans="1:112" ht="22.15" customHeight="1" thickTop="1">
@@ -5556,7 +5556,7 @@
       <c r="C14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="232" t="s">
+      <c r="D14" s="201" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="13"/>
@@ -5572,13 +5572,13 @@
       <c r="K14" s="166"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="225"/>
-      <c r="O14" s="225"/>
-      <c r="P14" s="225"/>
-      <c r="Q14" s="225"/>
-      <c r="R14" s="225"/>
-      <c r="S14" s="225"/>
-      <c r="T14" s="225"/>
+      <c r="N14" s="218"/>
+      <c r="O14" s="218"/>
+      <c r="P14" s="218"/>
+      <c r="Q14" s="218"/>
+      <c r="R14" s="218"/>
+      <c r="S14" s="218"/>
+      <c r="T14" s="218"/>
       <c r="U14" s="3"/>
       <c r="V14" s="166"/>
       <c r="W14" s="85" t="s">
@@ -5595,7 +5595,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="233"/>
+      <c r="D15" s="202"/>
       <c r="E15" s="13"/>
       <c r="G15" s="135"/>
       <c r="H15" s="82" t="s">
@@ -5608,13 +5608,13 @@
       <c r="K15" s="163"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="225"/>
-      <c r="O15" s="225"/>
-      <c r="P15" s="225"/>
-      <c r="Q15" s="225"/>
-      <c r="R15" s="225"/>
-      <c r="S15" s="225"/>
-      <c r="T15" s="225"/>
+      <c r="N15" s="218"/>
+      <c r="O15" s="218"/>
+      <c r="P15" s="218"/>
+      <c r="Q15" s="218"/>
+      <c r="R15" s="218"/>
+      <c r="S15" s="218"/>
+      <c r="T15" s="218"/>
       <c r="U15" s="3"/>
       <c r="V15" s="163"/>
       <c r="W15" s="85" t="s">
@@ -5642,13 +5642,13 @@
         <v>12</v>
       </c>
       <c r="K16" s="167"/>
-      <c r="N16" s="225"/>
-      <c r="O16" s="225"/>
-      <c r="P16" s="225"/>
-      <c r="Q16" s="225"/>
-      <c r="R16" s="225"/>
-      <c r="S16" s="225"/>
-      <c r="T16" s="225"/>
+      <c r="N16" s="218"/>
+      <c r="O16" s="218"/>
+      <c r="P16" s="218"/>
+      <c r="Q16" s="218"/>
+      <c r="R16" s="218"/>
+      <c r="S16" s="218"/>
+      <c r="T16" s="218"/>
       <c r="U16" s="3"/>
       <c r="V16" s="167"/>
       <c r="W16" s="86" t="s">
@@ -5667,23 +5667,23 @@
       <c r="C17" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="232" t="s">
+      <c r="D17" s="201" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="13"/>
       <c r="G17" s="137"/>
       <c r="H17" s="137"/>
       <c r="I17" s="129"/>
-      <c r="J17" s="244" t="s">
+      <c r="J17" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="244"/>
+      <c r="K17" s="198"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="244" t="s">
+      <c r="V17" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="W17" s="244"/>
+      <c r="W17" s="198"/>
       <c r="X17" s="130"/>
       <c r="Y17" s="130"/>
       <c r="Z17" s="4"/>
@@ -5693,12 +5693,12 @@
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="233"/>
+      <c r="D18" s="202"/>
       <c r="E18" s="13"/>
-      <c r="G18" s="229" t="s">
+      <c r="G18" s="199" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="229"/>
+      <c r="H18" s="199"/>
       <c r="I18" s="123" t="s">
         <v>70</v>
       </c>
@@ -5706,15 +5706,15 @@
         <f>K14</f>
         <v>0</v>
       </c>
-      <c r="O18" s="198"/>
-      <c r="P18" s="198"/>
-      <c r="Q18" s="198"/>
-      <c r="R18" s="198"/>
-      <c r="S18" s="198"/>
-      <c r="U18" s="229" t="s">
+      <c r="O18" s="242"/>
+      <c r="P18" s="242"/>
+      <c r="Q18" s="242"/>
+      <c r="R18" s="242"/>
+      <c r="S18" s="242"/>
+      <c r="U18" s="199" t="s">
         <v>30</v>
       </c>
-      <c r="V18" s="229"/>
+      <c r="V18" s="199"/>
       <c r="W18" s="123" t="s">
         <v>71</v>
       </c>
@@ -5745,11 +5745,11 @@
       <c r="K19" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="198"/>
-      <c r="P19" s="198"/>
-      <c r="Q19" s="198"/>
-      <c r="R19" s="198"/>
-      <c r="S19" s="198"/>
+      <c r="O19" s="242"/>
+      <c r="P19" s="242"/>
+      <c r="Q19" s="242"/>
+      <c r="R19" s="242"/>
+      <c r="S19" s="242"/>
       <c r="U19" s="90" t="s">
         <v>15</v>
       </c>
@@ -5774,7 +5774,7 @@
       <c r="C20" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="236" t="s">
+      <c r="D20" s="223" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="13"/>
@@ -5785,14 +5785,14 @@
       <c r="I20" s="168"/>
       <c r="J20" s="169"/>
       <c r="K20" s="168"/>
-      <c r="N20" s="209" t="s">
+      <c r="N20" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="198"/>
-      <c r="P20" s="198"/>
-      <c r="Q20" s="198"/>
-      <c r="R20" s="198"/>
-      <c r="S20" s="198"/>
+      <c r="O20" s="242"/>
+      <c r="P20" s="242"/>
+      <c r="Q20" s="242"/>
+      <c r="R20" s="242"/>
+      <c r="S20" s="242"/>
       <c r="U20" s="182">
         <v>1</v>
       </c>
@@ -5807,7 +5807,7 @@
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="237"/>
+      <c r="D21" s="224"/>
       <c r="E21" s="13"/>
       <c r="G21" s="182">
         <v>2</v>
@@ -5816,12 +5816,12 @@
       <c r="I21" s="168"/>
       <c r="J21" s="169"/>
       <c r="K21" s="168"/>
-      <c r="N21" s="209"/>
-      <c r="O21" s="198"/>
-      <c r="P21" s="198"/>
-      <c r="Q21" s="198"/>
-      <c r="R21" s="198"/>
-      <c r="S21" s="198"/>
+      <c r="N21" s="204"/>
+      <c r="O21" s="242"/>
+      <c r="P21" s="242"/>
+      <c r="Q21" s="242"/>
+      <c r="R21" s="242"/>
+      <c r="S21" s="242"/>
       <c r="U21" s="182">
         <v>2</v>
       </c>
@@ -5836,7 +5836,7 @@
       <c r="A22" s="12"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="237"/>
+      <c r="D22" s="224"/>
       <c r="E22" s="13"/>
       <c r="G22" s="182">
         <v>3</v>
@@ -5845,14 +5845,14 @@
       <c r="I22" s="168"/>
       <c r="J22" s="169"/>
       <c r="K22" s="168"/>
-      <c r="N22" s="208" t="s">
+      <c r="N22" s="229" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="208"/>
-      <c r="P22" s="208"/>
-      <c r="Q22" s="208"/>
-      <c r="R22" s="208"/>
-      <c r="S22" s="208"/>
+      <c r="O22" s="229"/>
+      <c r="P22" s="229"/>
+      <c r="Q22" s="229"/>
+      <c r="R22" s="229"/>
+      <c r="S22" s="229"/>
       <c r="U22" s="182">
         <v>3</v>
       </c>
@@ -5867,7 +5867,7 @@
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="237"/>
+      <c r="D23" s="224"/>
       <c r="E23" s="13"/>
       <c r="G23" s="182">
         <v>4</v>
@@ -5876,12 +5876,12 @@
       <c r="I23" s="168"/>
       <c r="J23" s="169"/>
       <c r="K23" s="168"/>
-      <c r="N23" s="208"/>
-      <c r="O23" s="208"/>
-      <c r="P23" s="208"/>
-      <c r="Q23" s="208"/>
-      <c r="R23" s="208"/>
-      <c r="S23" s="208"/>
+      <c r="N23" s="229"/>
+      <c r="O23" s="229"/>
+      <c r="P23" s="229"/>
+      <c r="Q23" s="229"/>
+      <c r="R23" s="229"/>
+      <c r="S23" s="229"/>
       <c r="U23" s="182">
         <v>4</v>
       </c>
@@ -5896,7 +5896,7 @@
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="237"/>
+      <c r="D24" s="224"/>
       <c r="E24" s="13"/>
       <c r="G24" s="182">
         <v>5</v>
@@ -5905,14 +5905,14 @@
       <c r="I24" s="168"/>
       <c r="J24" s="169"/>
       <c r="K24" s="168"/>
-      <c r="N24" s="217" t="s">
+      <c r="N24" s="210" t="s">
         <v>35</v>
       </c>
-      <c r="O24" s="218"/>
-      <c r="P24" s="218"/>
-      <c r="Q24" s="219"/>
-      <c r="R24" s="222"/>
-      <c r="S24" s="223"/>
+      <c r="O24" s="211"/>
+      <c r="P24" s="211"/>
+      <c r="Q24" s="212"/>
+      <c r="R24" s="215"/>
+      <c r="S24" s="216"/>
       <c r="U24" s="182">
         <v>5</v>
       </c>
@@ -5929,7 +5929,7 @@
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="237"/>
+      <c r="D25" s="224"/>
       <c r="E25" s="13"/>
       <c r="F25" s="91" t="s">
         <v>40</v>
@@ -5939,14 +5939,14 @@
       <c r="I25" s="185"/>
       <c r="J25" s="186"/>
       <c r="K25" s="186"/>
-      <c r="N25" s="217" t="s">
+      <c r="N25" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="O25" s="218"/>
-      <c r="P25" s="218"/>
-      <c r="Q25" s="219"/>
-      <c r="R25" s="220"/>
-      <c r="S25" s="221"/>
+      <c r="O25" s="211"/>
+      <c r="P25" s="211"/>
+      <c r="Q25" s="212"/>
+      <c r="R25" s="213"/>
+      <c r="S25" s="214"/>
       <c r="U25" s="183"/>
       <c r="V25" s="170"/>
       <c r="W25" s="170"/>
@@ -5961,18 +5961,18 @@
     <row r="26" spans="1:29">
       <c r="A26" s="9"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="237"/>
+      <c r="D26" s="224"/>
       <c r="G26" s="183"/>
       <c r="H26" s="184"/>
       <c r="I26" s="185"/>
       <c r="J26" s="186"/>
       <c r="K26" s="186"/>
-      <c r="N26" s="210"/>
-      <c r="O26" s="211"/>
-      <c r="P26" s="211"/>
-      <c r="Q26" s="211"/>
-      <c r="R26" s="211"/>
-      <c r="S26" s="212"/>
+      <c r="N26" s="230"/>
+      <c r="O26" s="231"/>
+      <c r="P26" s="231"/>
+      <c r="Q26" s="231"/>
+      <c r="R26" s="231"/>
+      <c r="S26" s="232"/>
       <c r="U26" s="183"/>
       <c r="V26" s="170"/>
       <c r="W26" s="170"/>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="9"/>
-      <c r="D27" s="237"/>
+      <c r="D27" s="224"/>
       <c r="G27" s="183"/>
       <c r="H27" s="184"/>
       <c r="I27" s="185"/>
@@ -6001,20 +6001,20 @@
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="9"/>
-      <c r="D28" s="237"/>
+      <c r="D28" s="224"/>
       <c r="G28" s="183"/>
       <c r="H28" s="184"/>
       <c r="I28" s="185"/>
       <c r="J28" s="186"/>
       <c r="K28" s="186"/>
-      <c r="N28" s="208" t="s">
+      <c r="N28" s="229" t="s">
         <v>52</v>
       </c>
-      <c r="O28" s="208"/>
-      <c r="P28" s="208"/>
-      <c r="Q28" s="208"/>
-      <c r="R28" s="208"/>
-      <c r="S28" s="208"/>
+      <c r="O28" s="229"/>
+      <c r="P28" s="229"/>
+      <c r="Q28" s="229"/>
+      <c r="R28" s="229"/>
+      <c r="S28" s="229"/>
       <c r="U28" s="183"/>
       <c r="V28" s="170"/>
       <c r="W28" s="170"/>
@@ -6025,18 +6025,18 @@
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="9"/>
-      <c r="D29" s="237"/>
+      <c r="D29" s="224"/>
       <c r="G29" s="183"/>
       <c r="H29" s="184"/>
       <c r="I29" s="185"/>
       <c r="J29" s="186"/>
       <c r="K29" s="186"/>
-      <c r="N29" s="208"/>
-      <c r="O29" s="208"/>
-      <c r="P29" s="208"/>
-      <c r="Q29" s="208"/>
-      <c r="R29" s="208"/>
-      <c r="S29" s="208"/>
+      <c r="N29" s="229"/>
+      <c r="O29" s="229"/>
+      <c r="P29" s="229"/>
+      <c r="Q29" s="229"/>
+      <c r="R29" s="229"/>
+      <c r="S29" s="229"/>
       <c r="U29" s="183"/>
       <c r="V29" s="170"/>
       <c r="W29" s="170"/>
@@ -6048,21 +6048,21 @@
     <row r="30" spans="1:29">
       <c r="A30" s="12"/>
       <c r="B30" s="13"/>
-      <c r="D30" s="238"/>
+      <c r="D30" s="225"/>
       <c r="E30" s="13"/>
       <c r="G30" s="183"/>
       <c r="H30" s="184"/>
       <c r="I30" s="185"/>
       <c r="J30" s="186"/>
       <c r="K30" s="186"/>
-      <c r="N30" s="213" t="s">
+      <c r="N30" s="236" t="s">
         <v>53</v>
       </c>
-      <c r="O30" s="214"/>
-      <c r="P30" s="214"/>
-      <c r="Q30" s="215"/>
-      <c r="R30" s="220"/>
-      <c r="S30" s="221"/>
+      <c r="O30" s="237"/>
+      <c r="P30" s="237"/>
+      <c r="Q30" s="238"/>
+      <c r="R30" s="213"/>
+      <c r="S30" s="214"/>
       <c r="U30" s="183"/>
       <c r="V30" s="170"/>
       <c r="W30" s="170"/>
@@ -6082,12 +6082,12 @@
       <c r="I31" s="185"/>
       <c r="J31" s="186"/>
       <c r="K31" s="186"/>
-      <c r="N31" s="210"/>
-      <c r="O31" s="211"/>
-      <c r="P31" s="211"/>
-      <c r="Q31" s="211"/>
-      <c r="R31" s="211"/>
-      <c r="S31" s="212"/>
+      <c r="N31" s="230"/>
+      <c r="O31" s="231"/>
+      <c r="P31" s="231"/>
+      <c r="Q31" s="231"/>
+      <c r="R31" s="231"/>
+      <c r="S31" s="232"/>
       <c r="U31" s="183"/>
       <c r="V31" s="170"/>
       <c r="W31" s="170"/>
@@ -6132,14 +6132,14 @@
       <c r="I33" s="185"/>
       <c r="J33" s="186"/>
       <c r="K33" s="186"/>
-      <c r="N33" s="199" t="s">
+      <c r="N33" s="233" t="s">
         <v>54</v>
       </c>
-      <c r="O33" s="200"/>
-      <c r="P33" s="200"/>
-      <c r="Q33" s="200"/>
-      <c r="R33" s="200"/>
-      <c r="S33" s="201"/>
+      <c r="O33" s="234"/>
+      <c r="P33" s="234"/>
+      <c r="Q33" s="234"/>
+      <c r="R33" s="234"/>
+      <c r="S33" s="235"/>
       <c r="U33" s="183"/>
       <c r="V33" s="170"/>
       <c r="W33" s="170"/>
@@ -6159,16 +6159,16 @@
       <c r="I34" s="185"/>
       <c r="J34" s="186"/>
       <c r="K34" s="186"/>
-      <c r="N34" s="202" t="s">
+      <c r="N34" s="243" t="s">
         <v>55</v>
       </c>
-      <c r="O34" s="203"/>
-      <c r="P34" s="204"/>
-      <c r="Q34" s="203" t="s">
+      <c r="O34" s="244"/>
+      <c r="P34" s="245"/>
+      <c r="Q34" s="244" t="s">
         <v>56</v>
       </c>
-      <c r="R34" s="203"/>
-      <c r="S34" s="204"/>
+      <c r="R34" s="244"/>
+      <c r="S34" s="245"/>
       <c r="U34" s="183"/>
       <c r="V34" s="170"/>
       <c r="W34" s="170"/>
@@ -6188,17 +6188,17 @@
       <c r="I35" s="185"/>
       <c r="J35" s="186"/>
       <c r="K35" s="186"/>
-      <c r="N35" s="205" t="s">
+      <c r="N35" s="226" t="s">
         <v>59</v>
       </c>
-      <c r="O35" s="206"/>
+      <c r="O35" s="227"/>
       <c r="P35" s="176">
         <v>3.15E-2</v>
       </c>
-      <c r="Q35" s="205" t="s">
+      <c r="Q35" s="226" t="s">
         <v>59</v>
       </c>
-      <c r="R35" s="206"/>
+      <c r="R35" s="227"/>
       <c r="S35" s="161">
         <v>2.8899999999999999E-2</v>
       </c>
@@ -6221,17 +6221,17 @@
       <c r="I36" s="185"/>
       <c r="J36" s="186"/>
       <c r="K36" s="186"/>
-      <c r="N36" s="205" t="s">
+      <c r="N36" s="226" t="s">
         <v>58</v>
       </c>
-      <c r="O36" s="206"/>
+      <c r="O36" s="227"/>
       <c r="P36" s="176">
         <v>3.49E-2</v>
       </c>
-      <c r="Q36" s="205" t="s">
+      <c r="Q36" s="226" t="s">
         <v>58</v>
       </c>
-      <c r="R36" s="206"/>
+      <c r="R36" s="227"/>
       <c r="S36" s="161">
         <v>3.0499999999999999E-2</v>
       </c>
@@ -6254,17 +6254,17 @@
       <c r="I37" s="185"/>
       <c r="J37" s="186"/>
       <c r="K37" s="186"/>
-      <c r="N37" s="205" t="s">
+      <c r="N37" s="226" t="s">
         <v>57</v>
       </c>
-      <c r="O37" s="206"/>
+      <c r="O37" s="227"/>
       <c r="P37" s="176">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="Q37" s="205" t="s">
+      <c r="Q37" s="226" t="s">
         <v>57</v>
       </c>
-      <c r="R37" s="206"/>
+      <c r="R37" s="227"/>
       <c r="S37" s="161">
         <v>3.5200000000000002E-2</v>
       </c>
@@ -6287,17 +6287,17 @@
       <c r="I38" s="185"/>
       <c r="J38" s="186"/>
       <c r="K38" s="186"/>
-      <c r="N38" s="205" t="s">
+      <c r="N38" s="226" t="s">
         <v>60</v>
       </c>
-      <c r="O38" s="206"/>
+      <c r="O38" s="227"/>
       <c r="P38" s="176">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="Q38" s="205" t="s">
+      <c r="Q38" s="226" t="s">
         <v>60</v>
       </c>
-      <c r="R38" s="206"/>
+      <c r="R38" s="227"/>
       <c r="S38" s="161">
         <v>3.6799999999999999E-2</v>
       </c>
@@ -6320,8 +6320,8 @@
       <c r="I39" s="185"/>
       <c r="J39" s="186"/>
       <c r="K39" s="186"/>
-      <c r="N39" s="196"/>
-      <c r="O39" s="197"/>
+      <c r="N39" s="240"/>
+      <c r="O39" s="241"/>
       <c r="P39" s="160"/>
       <c r="Q39" s="159"/>
       <c r="R39" s="159"/>
@@ -6370,14 +6370,14 @@
       <c r="I41" s="185"/>
       <c r="J41" s="186"/>
       <c r="K41" s="186"/>
-      <c r="N41" s="199" t="s">
+      <c r="N41" s="233" t="s">
         <v>63</v>
       </c>
-      <c r="O41" s="200"/>
-      <c r="P41" s="200"/>
-      <c r="Q41" s="200"/>
-      <c r="R41" s="200"/>
-      <c r="S41" s="201"/>
+      <c r="O41" s="234"/>
+      <c r="P41" s="234"/>
+      <c r="Q41" s="234"/>
+      <c r="R41" s="234"/>
+      <c r="S41" s="235"/>
       <c r="U41" s="183"/>
       <c r="V41" s="170"/>
       <c r="W41" s="170"/>
@@ -6397,16 +6397,16 @@
       <c r="I42" s="185"/>
       <c r="J42" s="186"/>
       <c r="K42" s="186"/>
-      <c r="N42" s="202" t="s">
+      <c r="N42" s="243" t="s">
         <v>62</v>
       </c>
-      <c r="O42" s="203"/>
-      <c r="P42" s="204"/>
-      <c r="Q42" s="203" t="s">
+      <c r="O42" s="244"/>
+      <c r="P42" s="245"/>
+      <c r="Q42" s="244" t="s">
         <v>61</v>
       </c>
-      <c r="R42" s="203"/>
-      <c r="S42" s="204"/>
+      <c r="R42" s="244"/>
+      <c r="S42" s="245"/>
       <c r="U42" s="183"/>
       <c r="V42" s="170"/>
       <c r="W42" s="170"/>
@@ -6426,8 +6426,8 @@
       <c r="I43" s="185"/>
       <c r="J43" s="186"/>
       <c r="K43" s="186"/>
-      <c r="N43" s="196"/>
-      <c r="O43" s="197"/>
+      <c r="N43" s="240"/>
+      <c r="O43" s="241"/>
       <c r="P43" s="160"/>
       <c r="Q43" s="159"/>
       <c r="R43" s="159"/>
@@ -10934,23 +10934,34 @@
       <c r="D377" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yAxQdGwXCQIt/yWV/q9dBkps7YH4zMpbo8ynwfsGqiPRx+TUYCj577aShIOjbV6jSwZsCn4rZWvwgMUQDhS+pQ==" saltValue="2nTIO7S2zE20MhYrzQe90g==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" sort="0" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xgLqzFxT9aQap/j46ZDvPwVddzalKVIOWjosGEVa+tUt+X+8afLq/dS+MAnNBk9bNML61V1xRn98kDFnJT8j8g==" saltValue="7OP1am2+UEyBV2T3R784yg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertHyperlinks="0" sort="0" autoFilter="0"/>
   <mergeCells count="57">
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="X7:Y9"/>
-    <mergeCell ref="X10:Y12"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="O18:S21"/>
+    <mergeCell ref="N41:S41"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="N22:S23"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N28:S29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N26:S26"/>
+    <mergeCell ref="N37:O37"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="N25:Q25"/>
     <mergeCell ref="R25:S25"/>
@@ -10967,32 +10978,21 @@
     <mergeCell ref="H10:I12"/>
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="D20:D30"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="N22:S23"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N28:S29"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="N26:S26"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="O18:S21"/>
-    <mergeCell ref="N41:S41"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="Q42:S42"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="X7:Y9"/>
+    <mergeCell ref="X10:Y12"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <conditionalFormatting sqref="X16">
     <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThan">
@@ -11092,12 +11092,12 @@
     <row r="2" spans="1:29" s="26" customFormat="1" ht="55.15" customHeight="1">
       <c r="A2" s="43"/>
       <c r="B2" s="47"/>
-      <c r="C2" s="261" t="s">
+      <c r="C2" s="256" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="262"/>
-      <c r="E2" s="262"/>
-      <c r="F2" s="262"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
       <c r="G2" s="48"/>
       <c r="H2" s="174"/>
       <c r="I2" s="174"/>
@@ -11132,10 +11132,10 @@
       <c r="E3" s="49"/>
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
-      <c r="H3" s="246" t="s">
+      <c r="H3" s="272" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="246"/>
+      <c r="I3" s="272"/>
       <c r="J3" s="173">
         <f>COUNTIF(G4:Z143,"ERROR")</f>
         <v>71</v>
@@ -11166,24 +11166,24 @@
       <c r="C4" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="268" t="s">
+      <c r="D4" s="265" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="48"/>
       <c r="G4" s="62"/>
-      <c r="H4" s="254" t="s">
+      <c r="H4" s="278" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="254"/>
-      <c r="J4" s="254">
+      <c r="I4" s="278"/>
+      <c r="J4" s="278">
         <f>COUNTIF(G6:Z143,"Correct")</f>
         <v>0</v>
       </c>
       <c r="K4" s="62"/>
       <c r="L4" s="62"/>
       <c r="M4" s="62"/>
-      <c r="N4" s="270" t="s">
+      <c r="N4" s="267" t="s">
         <v>24</v>
       </c>
       <c r="O4" s="68"/>
@@ -11206,17 +11206,17 @@
       <c r="A5" s="43"/>
       <c r="B5" s="47"/>
       <c r="C5" s="59"/>
-      <c r="D5" s="269"/>
+      <c r="D5" s="266"/>
       <c r="E5" s="47"/>
       <c r="F5" s="48"/>
       <c r="G5" s="54"/>
-      <c r="H5" s="254"/>
-      <c r="I5" s="254"/>
-      <c r="J5" s="254"/>
+      <c r="H5" s="278"/>
+      <c r="I5" s="278"/>
+      <c r="J5" s="278"/>
       <c r="K5" s="54"/>
       <c r="L5" s="54"/>
       <c r="M5" s="54"/>
-      <c r="N5" s="270"/>
+      <c r="N5" s="267"/>
       <c r="O5" s="68"/>
       <c r="P5" s="68"/>
       <c r="Q5" s="68"/>
@@ -11244,22 +11244,22 @@
       <c r="H6" s="54"/>
       <c r="I6" s="63"/>
       <c r="J6" s="54"/>
-      <c r="K6" s="276" t="s">
+      <c r="K6" s="247" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="54"/>
       <c r="M6" s="54"/>
-      <c r="N6" s="272" t="s">
+      <c r="N6" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="272"/>
-      <c r="P6" s="272"/>
-      <c r="Q6" s="272"/>
-      <c r="R6" s="272"/>
-      <c r="S6" s="272"/>
-      <c r="T6" s="272"/>
+      <c r="O6" s="269"/>
+      <c r="P6" s="269"/>
+      <c r="Q6" s="269"/>
+      <c r="R6" s="269"/>
+      <c r="S6" s="269"/>
+      <c r="T6" s="269"/>
       <c r="U6" s="54"/>
-      <c r="V6" s="276" t="s">
+      <c r="V6" s="247" t="s">
         <v>39</v>
       </c>
       <c r="W6" s="54"/>
@@ -11276,44 +11276,44 @@
       <c r="C7" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="268" t="s">
+      <c r="D7" s="265" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="48"/>
       <c r="G7" s="54"/>
-      <c r="H7" s="255" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="255"/>
+      <c r="H7" s="251" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="251"/>
       <c r="J7" s="66"/>
-      <c r="K7" s="276"/>
+      <c r="K7" s="247"/>
       <c r="L7" s="54"/>
       <c r="M7" s="54"/>
       <c r="N7" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="256" t="str">
+      <c r="O7" s="279" t="str">
         <f>IF(ISBLANK('Student Work'!O7:P7),"ERROR","Correct")</f>
         <v>ERROR</v>
       </c>
-      <c r="P7" s="257"/>
+      <c r="P7" s="280"/>
       <c r="Q7" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="258" t="str">
+      <c r="R7" s="270" t="str">
         <f>IF(ISBLANK('Student Work'!R7:S7),"ERROR","Correct")</f>
         <v>ERROR</v>
       </c>
-      <c r="S7" s="259"/>
+      <c r="S7" s="271"/>
       <c r="T7" s="193"/>
       <c r="U7" s="54"/>
-      <c r="V7" s="276"/>
+      <c r="V7" s="247"/>
       <c r="W7" s="54"/>
-      <c r="X7" s="255" t="s">
+      <c r="X7" s="251" t="s">
         <v>1</v>
       </c>
-      <c r="Y7" s="255"/>
+      <c r="Y7" s="251"/>
       <c r="Z7" s="54"/>
       <c r="AA7" s="54"/>
       <c r="AB7" s="54"/>
@@ -11323,12 +11323,12 @@
       <c r="A8" s="43"/>
       <c r="B8" s="47"/>
       <c r="C8" s="58"/>
-      <c r="D8" s="271"/>
+      <c r="D8" s="268"/>
       <c r="E8" s="47"/>
       <c r="F8" s="54"/>
       <c r="G8" s="54"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
+      <c r="H8" s="251"/>
+      <c r="I8" s="251"/>
       <c r="J8" s="140" t="s">
         <v>2</v>
       </c>
@@ -11341,19 +11341,19 @@
       <c r="N8" s="192" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="258" t="str">
+      <c r="O8" s="270" t="str">
         <f>IF(ISBLANK('Student Work'!O8:P8),"ERROR","Correct")</f>
         <v>ERROR</v>
       </c>
-      <c r="P8" s="259"/>
+      <c r="P8" s="271"/>
       <c r="Q8" s="192" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="258" t="str">
+      <c r="R8" s="270" t="str">
         <f>IF(ISBLANK('Student Work'!R8:S8),"ERROR","Correct")</f>
         <v>ERROR</v>
       </c>
-      <c r="S8" s="259"/>
+      <c r="S8" s="271"/>
       <c r="T8" s="151"/>
       <c r="U8" s="72"/>
       <c r="V8" s="110" t="str">
@@ -11363,8 +11363,8 @@
       <c r="W8" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="X8" s="255"/>
-      <c r="Y8" s="255"/>
+      <c r="X8" s="251"/>
+      <c r="Y8" s="251"/>
       <c r="Z8" s="54"/>
       <c r="AA8" s="54"/>
       <c r="AB8" s="54"/>
@@ -11374,12 +11374,12 @@
       <c r="A9" s="44"/>
       <c r="B9" s="53"/>
       <c r="C9" s="58"/>
-      <c r="D9" s="269"/>
+      <c r="D9" s="266"/>
       <c r="E9" s="53"/>
       <c r="F9" s="54"/>
       <c r="G9" s="54"/>
-      <c r="H9" s="255"/>
-      <c r="I9" s="255"/>
+      <c r="H9" s="251"/>
+      <c r="I9" s="251"/>
       <c r="J9" s="141" t="s">
         <v>5</v>
       </c>
@@ -11389,13 +11389,13 @@
       </c>
       <c r="L9" s="54"/>
       <c r="M9" s="54"/>
-      <c r="N9" s="260"/>
-      <c r="O9" s="260"/>
-      <c r="P9" s="260"/>
-      <c r="Q9" s="260"/>
-      <c r="R9" s="260"/>
-      <c r="S9" s="260"/>
-      <c r="T9" s="260"/>
+      <c r="N9" s="246"/>
+      <c r="O9" s="246"/>
+      <c r="P9" s="246"/>
+      <c r="Q9" s="246"/>
+      <c r="R9" s="246"/>
+      <c r="S9" s="246"/>
+      <c r="T9" s="246"/>
       <c r="U9" s="72"/>
       <c r="V9" s="108" t="str">
         <f>IF(AND(V8&lt;&gt;"ERROR",ABS('Student Work'!V9-0.06*'Student Work'!V8)&lt;0.02),"Correct","ERROR")</f>
@@ -11404,8 +11404,8 @@
       <c r="W9" s="146" t="s">
         <v>5</v>
       </c>
-      <c r="X9" s="255"/>
-      <c r="Y9" s="255"/>
+      <c r="X9" s="251"/>
+      <c r="Y9" s="251"/>
       <c r="Z9" s="54"/>
       <c r="AA9" s="54"/>
       <c r="AB9" s="54"/>
@@ -11419,8 +11419,8 @@
       <c r="E10" s="53"/>
       <c r="F10" s="65"/>
       <c r="G10" s="54"/>
-      <c r="H10" s="267"/>
-      <c r="I10" s="267"/>
+      <c r="H10" s="264"/>
+      <c r="I10" s="264"/>
       <c r="J10" s="141" t="s">
         <v>8</v>
       </c>
@@ -11430,13 +11430,13 @@
       </c>
       <c r="L10" s="54"/>
       <c r="M10" s="54"/>
-      <c r="N10" s="279"/>
-      <c r="O10" s="279"/>
-      <c r="P10" s="279"/>
-      <c r="Q10" s="279"/>
-      <c r="R10" s="279"/>
-      <c r="S10" s="279"/>
-      <c r="T10" s="279"/>
+      <c r="N10" s="254"/>
+      <c r="O10" s="254"/>
+      <c r="P10" s="254"/>
+      <c r="Q10" s="254"/>
+      <c r="R10" s="254"/>
+      <c r="S10" s="254"/>
+      <c r="T10" s="254"/>
       <c r="U10" s="72"/>
       <c r="V10" s="108" t="str">
         <f>IF(AND(NOT(ISBLANK('Student Work'!V10)),ABS('Student Work'!V10-('Student Work'!V8+'Student Work'!V9))&lt;0.01),"Correct","ERROR")</f>
@@ -11445,8 +11445,8 @@
       <c r="W10" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="X10" s="277"/>
-      <c r="Y10" s="277"/>
+      <c r="X10" s="250"/>
+      <c r="Y10" s="250"/>
       <c r="Z10" s="64"/>
       <c r="AA10" s="54"/>
       <c r="AB10" s="54"/>
@@ -11458,14 +11458,14 @@
       <c r="C11" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="273" t="s">
+      <c r="D11" s="248" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="65"/>
       <c r="G11" s="64"/>
-      <c r="H11" s="267"/>
-      <c r="I11" s="267"/>
+      <c r="H11" s="264"/>
+      <c r="I11" s="264"/>
       <c r="J11" s="141" t="s">
         <v>10</v>
       </c>
@@ -11475,13 +11475,13 @@
       </c>
       <c r="L11" s="54"/>
       <c r="M11" s="54"/>
-      <c r="N11" s="279"/>
-      <c r="O11" s="279"/>
-      <c r="P11" s="279"/>
-      <c r="Q11" s="279"/>
-      <c r="R11" s="279"/>
-      <c r="S11" s="279"/>
-      <c r="T11" s="279"/>
+      <c r="N11" s="254"/>
+      <c r="O11" s="254"/>
+      <c r="P11" s="254"/>
+      <c r="Q11" s="254"/>
+      <c r="R11" s="254"/>
+      <c r="S11" s="254"/>
+      <c r="T11" s="254"/>
       <c r="U11" s="72"/>
       <c r="V11" s="108" t="str">
         <f>IF(AND(NOT(ISBLANK('Student Work'!V11)),ABS('Student Work'!K10-'Student Work'!V11)&lt;0.01),"Correct","ERROR")</f>
@@ -11490,8 +11490,8 @@
       <c r="W11" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="X11" s="277"/>
-      <c r="Y11" s="277"/>
+      <c r="X11" s="250"/>
+      <c r="Y11" s="250"/>
       <c r="Z11" s="64"/>
       <c r="AA11" s="54"/>
       <c r="AB11" s="54"/>
@@ -11501,14 +11501,14 @@
       <c r="A12" s="44"/>
       <c r="B12" s="53"/>
       <c r="C12" s="57"/>
-      <c r="D12" s="274"/>
+      <c r="D12" s="249"/>
       <c r="E12" s="53"/>
-      <c r="F12" s="276" t="s">
+      <c r="F12" s="247" t="s">
         <v>72</v>
       </c>
       <c r="G12" s="64"/>
-      <c r="H12" s="267"/>
-      <c r="I12" s="267"/>
+      <c r="H12" s="264"/>
+      <c r="I12" s="264"/>
       <c r="J12" s="141" t="s">
         <v>9</v>
       </c>
@@ -11518,13 +11518,13 @@
       </c>
       <c r="L12" s="54"/>
       <c r="M12" s="54"/>
-      <c r="N12" s="279"/>
-      <c r="O12" s="279"/>
-      <c r="P12" s="279"/>
-      <c r="Q12" s="279"/>
-      <c r="R12" s="279"/>
-      <c r="S12" s="279"/>
-      <c r="T12" s="279"/>
+      <c r="N12" s="254"/>
+      <c r="O12" s="254"/>
+      <c r="P12" s="254"/>
+      <c r="Q12" s="254"/>
+      <c r="R12" s="254"/>
+      <c r="S12" s="254"/>
+      <c r="T12" s="254"/>
       <c r="U12" s="72"/>
       <c r="V12" s="111" t="str">
         <f>IF(AND(NOT(ISBLANK('Student Work'!V12)),ABS('Student Work'!V12-SUM('Student Work'!R30:S30))&lt;0.001),"Correct","ERROR")</f>
@@ -11533,9 +11533,9 @@
       <c r="W12" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="X12" s="277"/>
-      <c r="Y12" s="277"/>
-      <c r="Z12" s="276" t="s">
+      <c r="X12" s="250"/>
+      <c r="Y12" s="250"/>
+      <c r="Z12" s="247" t="s">
         <v>73</v>
       </c>
       <c r="AA12" s="54"/>
@@ -11548,7 +11548,7 @@
       <c r="C13" s="58"/>
       <c r="D13" s="55"/>
       <c r="E13" s="53"/>
-      <c r="F13" s="276"/>
+      <c r="F13" s="247"/>
       <c r="G13" s="64"/>
       <c r="H13" s="54"/>
       <c r="I13" s="54"/>
@@ -11561,13 +11561,13 @@
       </c>
       <c r="L13" s="54"/>
       <c r="M13" s="54"/>
-      <c r="N13" s="279"/>
-      <c r="O13" s="279"/>
-      <c r="P13" s="279"/>
-      <c r="Q13" s="279"/>
-      <c r="R13" s="279"/>
-      <c r="S13" s="279"/>
-      <c r="T13" s="279"/>
+      <c r="N13" s="254"/>
+      <c r="O13" s="254"/>
+      <c r="P13" s="254"/>
+      <c r="Q13" s="254"/>
+      <c r="R13" s="254"/>
+      <c r="S13" s="254"/>
+      <c r="T13" s="254"/>
       <c r="U13" s="72"/>
       <c r="V13" s="112" t="str">
         <f>IF(AND(NOT(ISBLANK('Student Work'!V13)),'Student Work'!V13='Student Work'!K13),"Correct","ERROR")</f>
@@ -11578,7 +11578,7 @@
       </c>
       <c r="X13" s="64"/>
       <c r="Y13" s="64"/>
-      <c r="Z13" s="276"/>
+      <c r="Z13" s="247"/>
       <c r="AA13" s="54"/>
       <c r="AB13" s="54"/>
       <c r="AC13" s="45"/>
@@ -11589,7 +11589,7 @@
       <c r="C14" s="115" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="273" t="s">
+      <c r="D14" s="248" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="53"/>
@@ -11611,13 +11611,13 @@
       </c>
       <c r="L14" s="69"/>
       <c r="M14" s="69"/>
-      <c r="N14" s="279"/>
-      <c r="O14" s="279"/>
-      <c r="P14" s="279"/>
-      <c r="Q14" s="279"/>
-      <c r="R14" s="279"/>
-      <c r="S14" s="279"/>
-      <c r="T14" s="279"/>
+      <c r="N14" s="254"/>
+      <c r="O14" s="254"/>
+      <c r="P14" s="254"/>
+      <c r="Q14" s="254"/>
+      <c r="R14" s="254"/>
+      <c r="S14" s="254"/>
+      <c r="T14" s="254"/>
       <c r="U14" s="72"/>
       <c r="V14" s="113" t="str">
         <f>IF(ISBLANK('Student Work'!V14),"ERROR",IF(ABS('Student Work'!V14-PMT('Student Work'!V12/12,'Student Work'!V13,'Student Work'!V11,-'Student Work'!V10))&lt;0.01,"Correct","ERROR"))</f>
@@ -11642,7 +11642,7 @@
       <c r="A15" s="44"/>
       <c r="B15" s="53"/>
       <c r="C15" s="56"/>
-      <c r="D15" s="274"/>
+      <c r="D15" s="249"/>
       <c r="E15" s="53"/>
       <c r="F15" s="54"/>
       <c r="G15" s="64"/>
@@ -11662,13 +11662,13 @@
       </c>
       <c r="L15" s="69"/>
       <c r="M15" s="69"/>
-      <c r="N15" s="279"/>
-      <c r="O15" s="279"/>
-      <c r="P15" s="279"/>
-      <c r="Q15" s="279"/>
-      <c r="R15" s="279"/>
-      <c r="S15" s="279"/>
-      <c r="T15" s="279"/>
+      <c r="N15" s="254"/>
+      <c r="O15" s="254"/>
+      <c r="P15" s="254"/>
+      <c r="Q15" s="254"/>
+      <c r="R15" s="254"/>
+      <c r="S15" s="254"/>
+      <c r="T15" s="254"/>
       <c r="U15" s="72"/>
       <c r="V15" s="108" t="str">
         <f>IF(ISBLANK('Student Work'!V15),"ERROR",IF(ABS('Student Work'!V15-'Student Work'!V14*'Student Work'!V13)&lt;1,"Correct","ERROR"))</f>
@@ -11713,13 +11713,13 @@
       </c>
       <c r="L16" s="54"/>
       <c r="M16" s="54"/>
-      <c r="N16" s="279"/>
-      <c r="O16" s="279"/>
-      <c r="P16" s="279"/>
-      <c r="Q16" s="279"/>
-      <c r="R16" s="279"/>
-      <c r="S16" s="279"/>
-      <c r="T16" s="279"/>
+      <c r="N16" s="254"/>
+      <c r="O16" s="254"/>
+      <c r="P16" s="254"/>
+      <c r="Q16" s="254"/>
+      <c r="R16" s="254"/>
+      <c r="S16" s="254"/>
+      <c r="T16" s="254"/>
       <c r="U16" s="72"/>
       <c r="V16" s="109" t="str">
         <f>IF(ISBLANK('Student Work'!V16),"ERROR",IF(ABS('Student Work'!V16-(FV('Student Work'!V12/12,'Student Work'!V13,-'Student Work'!V14,-'Student Work'!V11)-'Student Work'!X14))&lt;0.05,"Correct","ERROR"))</f>
@@ -11746,16 +11746,16 @@
       <c r="C17" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="273" t="s">
+      <c r="D17" s="248" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="H17" s="54"/>
-      <c r="I17" s="275"/>
-      <c r="J17" s="275"/>
-      <c r="K17" s="275"/>
+      <c r="I17" s="252"/>
+      <c r="J17" s="252"/>
+      <c r="K17" s="252"/>
       <c r="L17" s="54"/>
       <c r="M17" s="54"/>
       <c r="N17" s="54"/>
@@ -11768,9 +11768,9 @@
       <c r="U17" s="72"/>
       <c r="V17" s="70"/>
       <c r="W17" s="71"/>
-      <c r="X17" s="275"/>
-      <c r="Y17" s="275"/>
-      <c r="Z17" s="275"/>
+      <c r="X17" s="252"/>
+      <c r="Y17" s="252"/>
+      <c r="Z17" s="252"/>
       <c r="AA17" s="54"/>
       <c r="AB17" s="54"/>
       <c r="AC17" s="45"/>
@@ -11779,13 +11779,13 @@
       <c r="A18" s="44"/>
       <c r="B18" s="53"/>
       <c r="C18" s="55"/>
-      <c r="D18" s="274"/>
+      <c r="D18" s="249"/>
       <c r="E18" s="53"/>
       <c r="F18" s="54"/>
-      <c r="G18" s="278" t="s">
+      <c r="G18" s="253" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="278"/>
+      <c r="H18" s="253"/>
       <c r="I18" s="138" t="s">
         <v>44</v>
       </c>
@@ -11803,10 +11803,10 @@
       <c r="R18" s="54"/>
       <c r="S18" s="54"/>
       <c r="T18" s="54"/>
-      <c r="U18" s="280" t="s">
+      <c r="U18" s="255" t="s">
         <v>30</v>
       </c>
-      <c r="V18" s="280"/>
+      <c r="V18" s="255"/>
       <c r="W18" s="152"/>
       <c r="X18" s="74"/>
       <c r="Y18" s="54"/>
@@ -11872,7 +11872,7 @@
       <c r="C20" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="268" t="s">
+      <c r="D20" s="265" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="53"/>
@@ -11898,7 +11898,7 @@
       </c>
       <c r="L20" s="54"/>
       <c r="M20" s="54"/>
-      <c r="N20" s="276" t="s">
+      <c r="N20" s="247" t="s">
         <v>25</v>
       </c>
       <c r="O20" s="54"/>
@@ -11935,7 +11935,7 @@
       <c r="A21" s="44"/>
       <c r="B21" s="53"/>
       <c r="C21" s="53"/>
-      <c r="D21" s="271"/>
+      <c r="D21" s="268"/>
       <c r="E21" s="53"/>
       <c r="F21" s="54"/>
       <c r="G21" s="116">
@@ -11959,7 +11959,7 @@
       </c>
       <c r="L21" s="54"/>
       <c r="M21" s="54"/>
-      <c r="N21" s="276"/>
+      <c r="N21" s="247"/>
       <c r="O21" s="54"/>
       <c r="P21" s="54"/>
       <c r="Q21" s="54"/>
@@ -11994,7 +11994,7 @@
       <c r="A22" s="44"/>
       <c r="B22" s="53"/>
       <c r="C22" s="53"/>
-      <c r="D22" s="271"/>
+      <c r="D22" s="268"/>
       <c r="E22" s="53"/>
       <c r="F22" s="54"/>
       <c r="G22" s="116">
@@ -12018,14 +12018,14 @@
       </c>
       <c r="L22" s="54"/>
       <c r="M22" s="54"/>
-      <c r="N22" s="247" t="s">
+      <c r="N22" s="273" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="247"/>
-      <c r="P22" s="247"/>
-      <c r="Q22" s="247"/>
-      <c r="R22" s="247"/>
-      <c r="S22" s="247"/>
+      <c r="O22" s="273"/>
+      <c r="P22" s="273"/>
+      <c r="Q22" s="273"/>
+      <c r="R22" s="273"/>
+      <c r="S22" s="273"/>
       <c r="T22" s="54"/>
       <c r="U22" s="150">
         <v>3</v>
@@ -12055,7 +12055,7 @@
       <c r="A23" s="44"/>
       <c r="B23" s="53"/>
       <c r="C23" s="53"/>
-      <c r="D23" s="271"/>
+      <c r="D23" s="268"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54"/>
       <c r="G23" s="116">
@@ -12079,12 +12079,12 @@
       </c>
       <c r="L23" s="54"/>
       <c r="M23" s="54"/>
-      <c r="N23" s="248"/>
-      <c r="O23" s="248"/>
-      <c r="P23" s="248"/>
-      <c r="Q23" s="248"/>
-      <c r="R23" s="248"/>
-      <c r="S23" s="248"/>
+      <c r="N23" s="274"/>
+      <c r="O23" s="274"/>
+      <c r="P23" s="274"/>
+      <c r="Q23" s="274"/>
+      <c r="R23" s="274"/>
+      <c r="S23" s="274"/>
       <c r="T23" s="54"/>
       <c r="U23" s="150">
         <v>4</v>
@@ -12114,7 +12114,7 @@
       <c r="A24" s="44"/>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
-      <c r="D24" s="269"/>
+      <c r="D24" s="266"/>
       <c r="E24" s="53"/>
       <c r="F24" s="54"/>
       <c r="G24" s="116">
@@ -12138,17 +12138,17 @@
       </c>
       <c r="L24" s="54"/>
       <c r="M24" s="54"/>
-      <c r="N24" s="249" t="s">
+      <c r="N24" s="260" t="s">
         <v>35</v>
       </c>
-      <c r="O24" s="249"/>
-      <c r="P24" s="249"/>
-      <c r="Q24" s="251"/>
-      <c r="R24" s="252" t="str">
+      <c r="O24" s="260"/>
+      <c r="P24" s="260"/>
+      <c r="Q24" s="261"/>
+      <c r="R24" s="276" t="str">
         <f>IF(ISBLANK('Student Work'!R24:S24),"ERROR",IF('Student Work'!R24:S24&gt;0,IF('Student Work'!R24&gt;10,"Caution: Too Long!","Correct"),"ERROR"))</f>
         <v>ERROR</v>
       </c>
-      <c r="S24" s="253"/>
+      <c r="S24" s="277"/>
       <c r="T24" s="54"/>
       <c r="U24" s="150">
         <v>5</v>
@@ -12178,7 +12178,7 @@
       <c r="A25" s="44"/>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
-      <c r="D25" s="263" t="s">
+      <c r="D25" s="258" t="s">
         <v>69</v>
       </c>
       <c r="E25" s="53"/>
@@ -12207,17 +12207,17 @@
       </c>
       <c r="L25" s="54"/>
       <c r="M25" s="54"/>
-      <c r="N25" s="249" t="s">
+      <c r="N25" s="260" t="s">
         <v>36</v>
       </c>
-      <c r="O25" s="249"/>
-      <c r="P25" s="249"/>
-      <c r="Q25" s="251"/>
-      <c r="R25" s="265" t="str">
+      <c r="O25" s="260"/>
+      <c r="P25" s="260"/>
+      <c r="Q25" s="261"/>
+      <c r="R25" s="262" t="str">
         <f>IF(ISBLANK('Student Work'!R25:S25),"ERROR",IF(AND('Student Work'!R25:S25&gt;0,'Student Work'!R25:S25&lt;0.1),"Correct","ERROR"))</f>
         <v>ERROR</v>
       </c>
-      <c r="S25" s="266"/>
+      <c r="S25" s="263"/>
       <c r="T25" s="54"/>
       <c r="U25" s="107">
         <f>IF($V$13="Correct",IF(AND(U24+1&lt;='Student Work'!$V$13,U24&lt;&gt;0),U24+1,IF('Student Work'!U25&gt;0,"ERROR",0)),0)</f>
@@ -12250,7 +12250,7 @@
       <c r="A26" s="43"/>
       <c r="B26" s="47"/>
       <c r="C26" s="53"/>
-      <c r="D26" s="264"/>
+      <c r="D26" s="259"/>
       <c r="E26" s="47"/>
       <c r="F26" s="54"/>
       <c r="G26" s="107">
@@ -12275,12 +12275,12 @@
       </c>
       <c r="L26" s="54"/>
       <c r="M26" s="54"/>
-      <c r="N26" s="260"/>
-      <c r="O26" s="260"/>
-      <c r="P26" s="260"/>
-      <c r="Q26" s="260"/>
-      <c r="R26" s="260"/>
-      <c r="S26" s="260"/>
+      <c r="N26" s="246"/>
+      <c r="O26" s="246"/>
+      <c r="P26" s="246"/>
+      <c r="Q26" s="246"/>
+      <c r="R26" s="246"/>
+      <c r="S26" s="246"/>
       <c r="T26" s="54"/>
       <c r="U26" s="107">
         <f>IF($V$13="Correct",IF(AND(U25+1&lt;='Student Work'!$V$13,U25&lt;&gt;0),U25+1,IF('Student Work'!U26&gt;0,"ERROR",0)),0)</f>
@@ -12314,7 +12314,7 @@
       <c r="A27" s="43"/>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>
-      <c r="D27" s="264"/>
+      <c r="D27" s="259"/>
       <c r="E27" s="47"/>
       <c r="F27" s="54"/>
       <c r="G27" s="107">
@@ -12378,7 +12378,7 @@
       <c r="A28" s="43"/>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
-      <c r="D28" s="264"/>
+      <c r="D28" s="259"/>
       <c r="E28" s="47"/>
       <c r="F28" s="54"/>
       <c r="G28" s="107">
@@ -12403,14 +12403,14 @@
       </c>
       <c r="L28" s="54"/>
       <c r="M28" s="54"/>
-      <c r="N28" s="247" t="s">
+      <c r="N28" s="273" t="s">
         <v>52</v>
       </c>
-      <c r="O28" s="247"/>
-      <c r="P28" s="247"/>
-      <c r="Q28" s="247"/>
-      <c r="R28" s="247"/>
-      <c r="S28" s="247"/>
+      <c r="O28" s="273"/>
+      <c r="P28" s="273"/>
+      <c r="Q28" s="273"/>
+      <c r="R28" s="273"/>
+      <c r="S28" s="273"/>
       <c r="T28" s="54"/>
       <c r="U28" s="107">
         <f>IF($V$13="Correct",IF(AND(U27+1&lt;='Student Work'!$V$13,U27&lt;&gt;0),U27+1,IF('Student Work'!U28&gt;0,"ERROR",0)),0)</f>
@@ -12444,7 +12444,7 @@
       <c r="A29" s="43"/>
       <c r="B29" s="47"/>
       <c r="C29" s="47"/>
-      <c r="D29" s="264"/>
+      <c r="D29" s="259"/>
       <c r="E29" s="47"/>
       <c r="F29" s="54"/>
       <c r="G29" s="107">
@@ -12469,12 +12469,12 @@
       </c>
       <c r="L29" s="54"/>
       <c r="M29" s="54"/>
-      <c r="N29" s="248"/>
-      <c r="O29" s="248"/>
-      <c r="P29" s="248"/>
-      <c r="Q29" s="248"/>
-      <c r="R29" s="248"/>
-      <c r="S29" s="248"/>
+      <c r="N29" s="274"/>
+      <c r="O29" s="274"/>
+      <c r="P29" s="274"/>
+      <c r="Q29" s="274"/>
+      <c r="R29" s="274"/>
+      <c r="S29" s="274"/>
       <c r="T29" s="54"/>
       <c r="U29" s="107">
         <f>IF($V$13="Correct",IF(AND(U28+1&lt;='Student Work'!$V$13,U28&lt;&gt;0),U28+1,IF('Student Work'!U29&gt;0,"ERROR",0)),0)</f>
@@ -12508,7 +12508,7 @@
       <c r="A30" s="44"/>
       <c r="B30" s="53"/>
       <c r="C30" s="47"/>
-      <c r="D30" s="264"/>
+      <c r="D30" s="259"/>
       <c r="E30" s="53"/>
       <c r="F30" s="54"/>
       <c r="G30" s="107">
@@ -12533,17 +12533,17 @@
       </c>
       <c r="L30" s="54"/>
       <c r="M30" s="54"/>
-      <c r="N30" s="249" t="s">
+      <c r="N30" s="260" t="s">
         <v>53</v>
       </c>
-      <c r="O30" s="249"/>
-      <c r="P30" s="249"/>
-      <c r="Q30" s="249"/>
-      <c r="R30" s="250" t="str">
+      <c r="O30" s="260"/>
+      <c r="P30" s="260"/>
+      <c r="Q30" s="260"/>
+      <c r="R30" s="275" t="str">
         <f>IF(ISBLANK('Student Work'!R30:S30),"ERROR",IF(AND('Student Work'!R30:S30&gt;0,'Student Work'!R30:S30&lt;0.1),"Correct","ERROR"))</f>
         <v>ERROR</v>
       </c>
-      <c r="S30" s="250"/>
+      <c r="S30" s="275"/>
       <c r="T30" s="54"/>
       <c r="U30" s="107">
         <f>IF($V$13="Correct",IF(AND(U29+1&lt;='Student Work'!$V$13,U29&lt;&gt;0),U29+1,IF('Student Work'!U30&gt;0,"ERROR",0)),0)</f>
@@ -12577,7 +12577,7 @@
       <c r="A31" s="44"/>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
-      <c r="D31" s="264"/>
+      <c r="D31" s="259"/>
       <c r="E31" s="53"/>
       <c r="F31" s="54"/>
       <c r="G31" s="107">
@@ -12602,12 +12602,12 @@
       </c>
       <c r="L31" s="54"/>
       <c r="M31" s="54"/>
-      <c r="N31" s="260"/>
-      <c r="O31" s="260"/>
-      <c r="P31" s="260"/>
-      <c r="Q31" s="260"/>
-      <c r="R31" s="260"/>
-      <c r="S31" s="260"/>
+      <c r="N31" s="246"/>
+      <c r="O31" s="246"/>
+      <c r="P31" s="246"/>
+      <c r="Q31" s="246"/>
+      <c r="R31" s="246"/>
+      <c r="S31" s="246"/>
       <c r="T31" s="54"/>
       <c r="U31" s="107">
         <f>IF($V$13="Correct",IF(AND(U30+1&lt;='Student Work'!$V$13,U30&lt;&gt;0),U30+1,IF('Student Work'!U31&gt;0,"ERROR",0)),0)</f>
@@ -12641,7 +12641,7 @@
       <c r="A32" s="44"/>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
-      <c r="D32" s="264"/>
+      <c r="D32" s="259"/>
       <c r="E32" s="53"/>
       <c r="F32" s="54"/>
       <c r="G32" s="107">
@@ -12705,7 +12705,7 @@
       <c r="A33" s="44"/>
       <c r="B33" s="53"/>
       <c r="C33" s="53"/>
-      <c r="D33" s="264"/>
+      <c r="D33" s="259"/>
       <c r="E33" s="53"/>
       <c r="F33" s="54"/>
       <c r="G33" s="107">
@@ -12769,7 +12769,7 @@
       <c r="A34" s="44"/>
       <c r="B34" s="53"/>
       <c r="C34" s="53"/>
-      <c r="D34" s="264"/>
+      <c r="D34" s="259"/>
       <c r="E34" s="53"/>
       <c r="F34" s="54"/>
       <c r="G34" s="107">
@@ -12833,7 +12833,7 @@
       <c r="A35" s="44"/>
       <c r="B35" s="53"/>
       <c r="C35" s="53"/>
-      <c r="D35" s="264"/>
+      <c r="D35" s="259"/>
       <c r="E35" s="53"/>
       <c r="F35" s="54"/>
       <c r="G35" s="107">
@@ -12897,7 +12897,7 @@
       <c r="A36" s="44"/>
       <c r="B36" s="53"/>
       <c r="C36" s="53"/>
-      <c r="D36" s="264"/>
+      <c r="D36" s="259"/>
       <c r="E36" s="53"/>
       <c r="F36" s="54"/>
       <c r="G36" s="107">
@@ -12961,7 +12961,7 @@
       <c r="A37" s="44"/>
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
-      <c r="D37" s="264"/>
+      <c r="D37" s="259"/>
       <c r="E37" s="53"/>
       <c r="F37" s="54"/>
       <c r="G37" s="107">
@@ -13025,7 +13025,7 @@
       <c r="A38" s="44"/>
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
-      <c r="D38" s="264"/>
+      <c r="D38" s="259"/>
       <c r="E38" s="53"/>
       <c r="F38" s="54"/>
       <c r="G38" s="107">
@@ -13089,7 +13089,7 @@
       <c r="A39" s="44"/>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
-      <c r="D39" s="264"/>
+      <c r="D39" s="259"/>
       <c r="E39" s="53"/>
       <c r="F39" s="54"/>
       <c r="G39" s="107">
@@ -13153,7 +13153,7 @@
       <c r="A40" s="44"/>
       <c r="B40" s="53"/>
       <c r="C40" s="53"/>
-      <c r="D40" s="264"/>
+      <c r="D40" s="259"/>
       <c r="E40" s="53"/>
       <c r="F40" s="54"/>
       <c r="G40" s="107">
@@ -13217,7 +13217,7 @@
       <c r="A41" s="44"/>
       <c r="B41" s="53"/>
       <c r="C41" s="53"/>
-      <c r="D41" s="264"/>
+      <c r="D41" s="259"/>
       <c r="E41" s="53"/>
       <c r="F41" s="54"/>
       <c r="G41" s="107">
@@ -13281,7 +13281,7 @@
       <c r="A42" s="44"/>
       <c r="B42" s="53"/>
       <c r="C42" s="53"/>
-      <c r="D42" s="264"/>
+      <c r="D42" s="259"/>
       <c r="E42" s="53"/>
       <c r="F42" s="54"/>
       <c r="G42" s="107">
@@ -13345,7 +13345,7 @@
       <c r="A43" s="44"/>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
-      <c r="D43" s="264"/>
+      <c r="D43" s="259"/>
       <c r="E43" s="53"/>
       <c r="F43" s="54"/>
       <c r="G43" s="107">
@@ -13409,7 +13409,7 @@
       <c r="A44" s="44"/>
       <c r="B44" s="53"/>
       <c r="C44" s="53"/>
-      <c r="D44" s="264"/>
+      <c r="D44" s="259"/>
       <c r="E44" s="53"/>
       <c r="F44" s="54"/>
       <c r="G44" s="107">
@@ -13473,7 +13473,7 @@
       <c r="A45" s="44"/>
       <c r="B45" s="53"/>
       <c r="C45" s="53"/>
-      <c r="D45" s="264"/>
+      <c r="D45" s="259"/>
       <c r="E45" s="53"/>
       <c r="F45" s="54"/>
       <c r="G45" s="107">
@@ -13537,7 +13537,7 @@
       <c r="A46" s="44"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
-      <c r="D46" s="264"/>
+      <c r="D46" s="259"/>
       <c r="E46" s="53"/>
       <c r="F46" s="54"/>
       <c r="G46" s="107">
@@ -13601,7 +13601,7 @@
       <c r="A47" s="44"/>
       <c r="B47" s="53"/>
       <c r="C47" s="53"/>
-      <c r="D47" s="264"/>
+      <c r="D47" s="259"/>
       <c r="E47" s="53"/>
       <c r="F47" s="54"/>
       <c r="G47" s="107">
@@ -13665,7 +13665,7 @@
       <c r="A48" s="44"/>
       <c r="B48" s="53"/>
       <c r="C48" s="53"/>
-      <c r="D48" s="264"/>
+      <c r="D48" s="259"/>
       <c r="E48" s="53"/>
       <c r="F48" s="54"/>
       <c r="G48" s="107">
@@ -13729,7 +13729,7 @@
       <c r="A49" s="44"/>
       <c r="B49" s="53"/>
       <c r="C49" s="53"/>
-      <c r="D49" s="264"/>
+      <c r="D49" s="259"/>
       <c r="E49" s="53"/>
       <c r="F49" s="54"/>
       <c r="G49" s="107">
@@ -13793,7 +13793,7 @@
       <c r="A50" s="44"/>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
-      <c r="D50" s="264"/>
+      <c r="D50" s="259"/>
       <c r="E50" s="53"/>
       <c r="F50" s="54"/>
       <c r="G50" s="107">
@@ -13857,7 +13857,7 @@
       <c r="A51" s="44"/>
       <c r="B51" s="54"/>
       <c r="C51" s="54"/>
-      <c r="D51" s="264"/>
+      <c r="D51" s="259"/>
       <c r="E51" s="54"/>
       <c r="F51" s="54"/>
       <c r="G51" s="107">
@@ -13921,7 +13921,7 @@
       <c r="A52" s="44"/>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
-      <c r="D52" s="264"/>
+      <c r="D52" s="259"/>
       <c r="E52" s="54"/>
       <c r="F52" s="54"/>
       <c r="G52" s="107">
@@ -13985,7 +13985,7 @@
       <c r="A53" s="44"/>
       <c r="B53" s="54"/>
       <c r="C53" s="54"/>
-      <c r="D53" s="264"/>
+      <c r="D53" s="259"/>
       <c r="E53" s="54"/>
       <c r="F53" s="54"/>
       <c r="G53" s="107">
@@ -22395,19 +22395,19 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="pOSsp7gPedbH9g4ZfV7rlhWJ/FTyqh/1oTKVGABpB1KIDw7k4uYahj20zRgEceuoKveRI9FWPj7Cdlej6xgC6g==" saltValue="kBVXPjpfUPepo5Pg4/WOAA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="42">
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="X10:Y12"/>
-    <mergeCell ref="X7:Y9"/>
-    <mergeCell ref="X17:Z17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="N10:T16"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="Z12:Z13"/>
-    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N28:S29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="N22:S23"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="H4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="H7:I9"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="N9:T9"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="D25:D53"/>
     <mergeCell ref="N25:Q25"/>
@@ -22424,19 +22424,19 @@
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="R8:S8"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N28:S29"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="N22:S23"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="H4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="H7:I9"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="N9:T9"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="X10:Y12"/>
+    <mergeCell ref="X7:Y9"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="N10:T16"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="Z12:Z13"/>
+    <mergeCell ref="V6:V7"/>
   </mergeCells>
   <conditionalFormatting sqref="G7:Z8 G17:Z17 G9:N10 G11:M16 U9:Z11 W18:Z18 G25:U25 W25:Y25 T18:U18 T19:Z19 G18:S19 G22:Z24 U26:U144 G26:T143 W26:Z143 U14:Z16 U12:Y13 G20:M21 O20:Z21">
     <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Caution">
@@ -22529,12 +22529,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22722,15 +22719,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17FF9E1A-0C09-452E-98F2-D8C646CB09C3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5F269E0-F682-472C-A86C-2C0D406473F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0acb5147-8577-475e-9c5c-8643af49afee"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22754,17 +22762,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5F269E0-F682-472C-A86C-2C0D406473F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17FF9E1A-0C09-452E-98F2-D8C646CB09C3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0acb5147-8577-475e-9c5c-8643af49afee"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>